<commit_message>
Update program URL references and enhance program ranking display in various components
</commit_message>
<xml_diff>
--- a/MBA Options_25.09.2025.xlsx
+++ b/MBA Options_25.09.2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Desktop\Kareer Studio\Upto Login\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Desktop\Kareer Studio\CORE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69FC7EF-10E3-46B8-9AE0-6FD70831D5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BF6B55-9E4E-452A-8203-3B928BC9EE50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$L$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$K$43</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>Serial No.</t>
   </si>
@@ -31,15 +31,9 @@
     <t>University</t>
   </si>
   <si>
-    <t>University Ranking</t>
-  </si>
-  <si>
     <t>Program Name</t>
   </si>
   <si>
-    <t>Website URL</t>
-  </si>
-  <si>
     <t>Campus</t>
   </si>
   <si>
@@ -73,12 +67,6 @@
     <t>University of East London</t>
   </si>
   <si>
-    <t>Webometrics World Ranking - 1357
-Webometrics National Ranking - 91
-US News Ranking - NA
-QS Ranking - 901</t>
-  </si>
-  <si>
     <t>MBA Master of Business Administration (Business Analytics) with Placement Year</t>
   </si>
   <si>
@@ -104,13 +92,31 @@
   </si>
   <si>
     <t>GBP 50</t>
+  </si>
+  <si>
+    <t>Webometrics World</t>
+  </si>
+  <si>
+    <t>Webometrics National</t>
+  </si>
+  <si>
+    <t>US News</t>
+  </si>
+  <si>
+    <t>QS Ranking</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Program Link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -124,6 +130,10 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -476,31 +486,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8" style="3" customWidth="1"/>
     <col min="2" max="2" width="44.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.44140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="38.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="50" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="13.109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.88671875" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="3"/>
+    <col min="3" max="3" width="38.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="50" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="15" width="17.88671875" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -511,152 +520,188 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="L1" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="57.6">
+        <v>23</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="2" customFormat="1" ht="28.8">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="4">
+        <v>6</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="4">
-        <v>6</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="57.6">
+      <c r="L2" s="4">
+        <v>23</v>
+      </c>
+      <c r="M2" s="4">
+        <v>5</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="2" customFormat="1" ht="28.8">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="4">
+        <v>6</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="4">
+      <c r="K3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="4">
+        <v>45</v>
+      </c>
+      <c r="M3" s="4">
         <v>6</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" ht="57.6">
+      <c r="N3" s="4">
+        <v>77</v>
+      </c>
+      <c r="O3" s="4">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="2" customFormat="1" ht="28.8">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="I4" s="4">
         <v>6</v>
       </c>
+      <c r="J4" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="K4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="2" customFormat="1">
+        <v>17</v>
+      </c>
+      <c r="L4" s="4">
+        <v>43</v>
+      </c>
+      <c r="M4" s="4">
+        <v>34</v>
+      </c>
+      <c r="N4" s="4">
+        <v>34</v>
+      </c>
+      <c r="O4" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="2" customFormat="1">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -665,12 +710,15 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
-    </row>
-    <row r="6" spans="1:12" s="2" customFormat="1">
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+    </row>
+    <row r="6" spans="1:15" s="2" customFormat="1">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -679,8 +727,11 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-    </row>
-    <row r="7" spans="1:12" s="2" customFormat="1">
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+    </row>
+    <row r="7" spans="1:15" s="2" customFormat="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -693,12 +744,15 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-    </row>
-    <row r="8" spans="1:12" s="2" customFormat="1">
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+    </row>
+    <row r="8" spans="1:15" s="2" customFormat="1">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -707,8 +761,11 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-    </row>
-    <row r="9" spans="1:12" s="2" customFormat="1">
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="1:15" s="2" customFormat="1">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -721,8 +778,11 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" s="2" customFormat="1">
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+    </row>
+    <row r="10" spans="1:15" s="2" customFormat="1">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -735,8 +795,11 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" s="2" customFormat="1">
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+    </row>
+    <row r="11" spans="1:15" s="2" customFormat="1">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -749,8 +812,11 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-    </row>
-    <row r="12" spans="1:12" s="2" customFormat="1">
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+    </row>
+    <row r="12" spans="1:15" s="2" customFormat="1">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -763,8 +829,11 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-    </row>
-    <row r="13" spans="1:12" s="2" customFormat="1">
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="1:15" s="2" customFormat="1">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -777,12 +846,15 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-    </row>
-    <row r="14" spans="1:12" s="2" customFormat="1">
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+    </row>
+    <row r="14" spans="1:15" s="2" customFormat="1">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -791,12 +863,15 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-    </row>
-    <row r="15" spans="1:12" s="2" customFormat="1">
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+    </row>
+    <row r="15" spans="1:15" s="2" customFormat="1">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -805,12 +880,15 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-    </row>
-    <row r="16" spans="1:12" s="2" customFormat="1">
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+    </row>
+    <row r="16" spans="1:15" s="2" customFormat="1">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -819,12 +897,15 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-    </row>
-    <row r="17" spans="1:12" s="2" customFormat="1">
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+    </row>
+    <row r="17" spans="1:15" s="2" customFormat="1">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -833,12 +914,15 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-    </row>
-    <row r="18" spans="1:12" s="2" customFormat="1">
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+    </row>
+    <row r="18" spans="1:15" s="2" customFormat="1">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -847,8 +931,11 @@
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
-    </row>
-    <row r="19" spans="1:12" s="2" customFormat="1">
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+    </row>
+    <row r="19" spans="1:15" s="2" customFormat="1">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -861,8 +948,11 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-    </row>
-    <row r="20" spans="1:12" s="2" customFormat="1">
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+    </row>
+    <row r="20" spans="1:15" s="2" customFormat="1">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -875,8 +965,11 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-    </row>
-    <row r="21" spans="1:12" s="2" customFormat="1">
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+    </row>
+    <row r="21" spans="1:15" s="2" customFormat="1">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -889,8 +982,11 @@
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
-    </row>
-    <row r="22" spans="1:12" s="2" customFormat="1">
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+    </row>
+    <row r="22" spans="1:15" s="2" customFormat="1">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -903,12 +999,15 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
-    </row>
-    <row r="23" spans="1:12" s="2" customFormat="1">
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+    </row>
+    <row r="23" spans="1:15" s="2" customFormat="1">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -917,12 +1016,15 @@
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
-    </row>
-    <row r="24" spans="1:12" s="2" customFormat="1">
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+    </row>
+    <row r="24" spans="1:15" s="2" customFormat="1">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -931,12 +1033,15 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
-    </row>
-    <row r="25" spans="1:12" s="2" customFormat="1">
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+    </row>
+    <row r="25" spans="1:15" s="2" customFormat="1">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -945,8 +1050,11 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
-    </row>
-    <row r="26" spans="1:12" s="2" customFormat="1">
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+    </row>
+    <row r="26" spans="1:15" s="2" customFormat="1">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -959,12 +1067,15 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
-    </row>
-    <row r="27" spans="1:12" s="2" customFormat="1">
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+    </row>
+    <row r="27" spans="1:15" s="2" customFormat="1">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -973,12 +1084,15 @@
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
-    </row>
-    <row r="28" spans="1:12" s="2" customFormat="1">
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+    </row>
+    <row r="28" spans="1:15" s="2" customFormat="1">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -987,12 +1101,15 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
-    </row>
-    <row r="29" spans="1:12" s="2" customFormat="1">
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+    </row>
+    <row r="29" spans="1:15" s="2" customFormat="1">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
@@ -1001,12 +1118,15 @@
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
-    </row>
-    <row r="30" spans="1:12" s="2" customFormat="1">
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+    </row>
+    <row r="30" spans="1:15" s="2" customFormat="1">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -1015,12 +1135,15 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
-    </row>
-    <row r="31" spans="1:12" s="2" customFormat="1">
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+    </row>
+    <row r="31" spans="1:15" s="2" customFormat="1">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -1029,12 +1152,15 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
-    </row>
-    <row r="32" spans="1:12" s="2" customFormat="1">
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+    </row>
+    <row r="32" spans="1:15" s="2" customFormat="1">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -1043,8 +1169,11 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
-    </row>
-    <row r="33" spans="1:12" s="2" customFormat="1">
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+    </row>
+    <row r="33" spans="1:15" s="2" customFormat="1">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1057,8 +1186,11 @@
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
-    </row>
-    <row r="34" spans="1:12" s="2" customFormat="1">
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+    </row>
+    <row r="34" spans="1:15" s="2" customFormat="1">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1071,8 +1203,11 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
-    </row>
-    <row r="35" spans="1:12" s="2" customFormat="1">
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+    </row>
+    <row r="35" spans="1:15" s="2" customFormat="1">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1085,12 +1220,15 @@
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
-    </row>
-    <row r="36" spans="1:12" s="2" customFormat="1">
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+    </row>
+    <row r="36" spans="1:15" s="2" customFormat="1">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -1099,12 +1237,15 @@
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
-    </row>
-    <row r="37" spans="1:12" s="2" customFormat="1">
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+    </row>
+    <row r="37" spans="1:15" s="2" customFormat="1">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -1113,8 +1254,11 @@
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
-    </row>
-    <row r="38" spans="1:12" s="2" customFormat="1">
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+    </row>
+    <row r="38" spans="1:15" s="2" customFormat="1">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1127,8 +1271,11 @@
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
-    </row>
-    <row r="39" spans="1:12" s="2" customFormat="1">
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+    </row>
+    <row r="39" spans="1:15" s="2" customFormat="1">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1141,8 +1288,11 @@
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
-    </row>
-    <row r="40" spans="1:12" s="2" customFormat="1">
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+    </row>
+    <row r="40" spans="1:15" s="2" customFormat="1">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1155,8 +1305,11 @@
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
-    </row>
-    <row r="41" spans="1:12" s="2" customFormat="1">
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+    </row>
+    <row r="41" spans="1:15" s="2" customFormat="1">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1169,8 +1322,11 @@
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
-    </row>
-    <row r="42" spans="1:12" s="2" customFormat="1">
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+    </row>
+    <row r="42" spans="1:15" s="2" customFormat="1">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1183,12 +1339,15 @@
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
-    </row>
-    <row r="43" spans="1:12" s="2" customFormat="1">
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+    </row>
+    <row r="43" spans="1:15" s="2" customFormat="1">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -1197,8 +1356,13 @@
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>